<commit_message>
Translating to English and fixing issues with readme.md
</commit_message>
<xml_diff>
--- a/configs/Investigadores y Ayudantes.xlsx
+++ b/configs/Investigadores y Ayudantes.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63F0D23-D403-4974-AA98-BEE31F1FDB0F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{F63F0D23-D403-4974-AA98-BEE31F1FDB0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9119EB3E-53E9-4E68-B840-6A1C83042EB8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,44 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
-  <si>
-    <t>Iván Aguas</t>
-  </si>
-  <si>
-    <t>xavier.aguas@epn.edu.ec</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>EPN</t>
   </si>
   <si>
-    <t>Alex Chamba</t>
-  </si>
-  <si>
-    <t>leimer.chamba@epn.edu.ec</t>
-  </si>
-  <si>
-    <t>Angel Alcócer</t>
-  </si>
-  <si>
-    <t>angel.alcocer.sep@hotmail.com</t>
-  </si>
-  <si>
-    <t>Luis Pacheco</t>
-  </si>
-  <si>
-    <t>luis.pacheco02@epn.edu.ec</t>
-  </si>
-  <si>
-    <t>Lenin Ibarra</t>
-  </si>
-  <si>
-    <t>lenin.ibarra@epn.edu.ec</t>
-  </si>
-  <si>
-    <t>jessica.zapata@epn.edu.ec</t>
-  </si>
-  <si>
     <t>Lorena Barona</t>
   </si>
   <si>
@@ -70,123 +37,12 @@
     <t>angel.valdivieso@epn.edu.ec</t>
   </si>
   <si>
-    <t>Freddy Benalcázar</t>
-  </si>
-  <si>
-    <t>fg.benalcazar@uta.edu.ec</t>
-  </si>
-  <si>
-    <t>UTA</t>
-  </si>
-  <si>
-    <t>re.nogales@uta.edu.ec</t>
-  </si>
-  <si>
-    <t>Jaime Guilcapi</t>
-  </si>
-  <si>
-    <t>jr.guilcapi@uta.edu.ec</t>
-  </si>
-  <si>
-    <t>Bryan Toalumbo</t>
-  </si>
-  <si>
-    <t>bryan.david.050@gmail.com</t>
-  </si>
-  <si>
-    <t>Ronnie Martínez</t>
-  </si>
-  <si>
-    <t>mronni17@gmail.com</t>
-  </si>
-  <si>
-    <t>Alexis Palate</t>
-  </si>
-  <si>
-    <t>alexisfuhrer0420@gmail.com</t>
-  </si>
-  <si>
-    <t>Mauricio Pérez</t>
-  </si>
-  <si>
-    <t>mperez1668@uta.edu.ec</t>
-  </si>
-  <si>
-    <t>Mauricio Dávalos</t>
-  </si>
-  <si>
-    <t>madvalosj@espe.edu.ec</t>
-  </si>
-  <si>
-    <t>ESPE</t>
-  </si>
-  <si>
-    <t>Jairo Espinoza</t>
-  </si>
-  <si>
-    <t>jhespinoza@espe.edu.ec</t>
-  </si>
-  <si>
-    <t>Marcelo Alvarez</t>
-  </si>
-  <si>
-    <t>rmalvarez@espe.edu.ec</t>
-  </si>
-  <si>
-    <t>0995678733</t>
-  </si>
-  <si>
-    <t>0995811242</t>
-  </si>
-  <si>
-    <t>0979085810</t>
-  </si>
-  <si>
-    <t>0981288316</t>
-  </si>
-  <si>
-    <t>0992176672</t>
-  </si>
-  <si>
-    <t>0998061535</t>
-  </si>
-  <si>
     <t>0987800285</t>
   </si>
   <si>
     <t>0984339279</t>
   </si>
   <si>
-    <t>0984026615</t>
-  </si>
-  <si>
-    <t>0996372410</t>
-  </si>
-  <si>
-    <t>0999915230</t>
-  </si>
-  <si>
-    <t>0962685361</t>
-  </si>
-  <si>
-    <t>0999935148</t>
-  </si>
-  <si>
-    <t>0968285305</t>
-  </si>
-  <si>
-    <t>0980446601</t>
-  </si>
-  <si>
-    <t>0983344522</t>
-  </si>
-  <si>
-    <t>0987515300</t>
-  </si>
-  <si>
-    <t>0992668556</t>
-  </si>
-  <si>
     <t>Marco E. Benalcázar</t>
   </si>
   <si>
@@ -208,12 +64,6 @@
     <t>Institución</t>
   </si>
   <si>
-    <t>Rubén Nogales</t>
-  </si>
-  <si>
-    <t>Jéssica Zapata</t>
-  </si>
-  <si>
     <t>Jonathan Zea</t>
   </si>
   <si>
@@ -230,6 +80,63 @@
   </si>
   <si>
     <t>0958789803</t>
+  </si>
+  <si>
+    <t>Victor Vimos</t>
+  </si>
+  <si>
+    <t>victor.vimos@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>Juan Pablo Vasconez</t>
+  </si>
+  <si>
+    <t>juan.vasconez@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>Alex Chico</t>
+  </si>
+  <si>
+    <t>Danny Díaz</t>
+  </si>
+  <si>
+    <t>Ricardo Romero</t>
+  </si>
+  <si>
+    <t>alex.chico@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>ricardo.romero@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>danny.diaz@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>0983489633</t>
+  </si>
+  <si>
+    <t>0998089858</t>
+  </si>
+  <si>
+    <t>0978860651</t>
+  </si>
+  <si>
+    <t>0978654041</t>
+  </si>
+  <si>
+    <t>0991624028</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>mail</t>
+  </si>
+  <si>
+    <t>celphone</t>
+  </si>
+  <si>
+    <t>U</t>
   </si>
 </sst>
 </file>
@@ -288,7 +195,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -298,9 +205,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -579,335 +492,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="8" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>60</v>
+        <v>11</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>42</v>
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>43</v>
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>44</v>
+        <v>27</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>45</v>
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>46</v>
+        <v>28</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{8BD40952-1AF5-4728-A055-B23B8F6F34D3}"/>
-    <hyperlink ref="B21" r:id="rId2" xr:uid="{A75EFE50-A6A3-4751-960D-30DE377C7AF2}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{8BD40952-1AF5-4728-A055-B23B8F6F34D3}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{A75EFE50-A6A3-4751-960D-30DE377C7AF2}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{5A6A673A-F807-4392-AB3D-53386085A02B}"/>
+    <hyperlink ref="B9" r:id="rId4" xr:uid="{3F272052-19AB-4259-9A3F-9B9E950F177A}"/>
+    <hyperlink ref="B11" r:id="rId5" xr:uid="{C4801EF3-5848-4AF1-95CD-892953B6FC13}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating list of new segmentators
</commit_message>
<xml_diff>
--- a/configs/Investigadores y Ayudantes.xlsx
+++ b/configs/Investigadores y Ayudantes.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{F63F0D23-D403-4974-AA98-BEE31F1FDB0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9119EB3E-53E9-4E68-B840-6A1C83042EB8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F065F6E0-7361-4D67-87FE-5A7A7E6CBBF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,38 +20,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="99">
   <si>
     <t>EPN</t>
   </si>
   <si>
-    <t>Lorena Barona</t>
-  </si>
-  <si>
     <t>lorena.barona@epn.edu.ec</t>
   </si>
   <si>
-    <t>Leonardo Valdivieso</t>
-  </si>
-  <si>
     <t>angel.valdivieso@epn.edu.ec</t>
   </si>
   <si>
-    <t>0987800285</t>
-  </si>
-  <si>
-    <t>0984339279</t>
-  </si>
-  <si>
-    <t>Marco E. Benalcázar</t>
-  </si>
-  <si>
     <t>marco.benalcazar@epn.edu.ec</t>
   </si>
   <si>
-    <t>0998458271</t>
-  </si>
-  <si>
     <t>Nombre</t>
   </si>
   <si>
@@ -64,45 +46,15 @@
     <t>Institución</t>
   </si>
   <si>
-    <t>Jonathan Zea</t>
-  </si>
-  <si>
-    <t>0999000683</t>
-  </si>
-  <si>
-    <t>z_tjalezea@yahoo.com</t>
-  </si>
-  <si>
-    <t>Francis Ferri</t>
-  </si>
-  <si>
     <t>francis.ferri@epn.edu.ec</t>
   </si>
   <si>
-    <t>0958789803</t>
-  </si>
-  <si>
-    <t>Victor Vimos</t>
-  </si>
-  <si>
     <t>victor.vimos@epn.edu.ec</t>
   </si>
   <si>
-    <t>Juan Pablo Vasconez</t>
-  </si>
-  <si>
     <t>juan.vasconez@epn.edu.ec</t>
   </si>
   <si>
-    <t>Alex Chico</t>
-  </si>
-  <si>
-    <t>Danny Díaz</t>
-  </si>
-  <si>
-    <t>Ricardo Romero</t>
-  </si>
-  <si>
     <t>alex.chico@epn.edu.ec</t>
   </si>
   <si>
@@ -112,57 +64,269 @@
     <t>danny.diaz@epn.edu.ec</t>
   </si>
   <si>
-    <t>0983489633</t>
-  </si>
-  <si>
-    <t>0998089858</t>
-  </si>
-  <si>
-    <t>0978860651</t>
-  </si>
-  <si>
-    <t>0978654041</t>
-  </si>
-  <si>
-    <t>0991624028</t>
-  </si>
-  <si>
     <t>other</t>
   </si>
   <si>
-    <t>mail</t>
-  </si>
-  <si>
-    <t>celphone</t>
-  </si>
-  <si>
     <t>U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jeimmy.eche@epn.edu.ec </t>
+  </si>
+  <si>
+    <t>sergio.guaman@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>veronica.zuniga@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>anthony.plua@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>byron.ortiz@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>diego.arias@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>jorge.martinez02@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>unkown mail</t>
+  </si>
+  <si>
+    <t>no celphone</t>
+  </si>
+  <si>
+    <t>pablo.flores01@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>ivanna.cevallos@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>kharol.chicaiza@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>dayana.guacapina@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>jonathan.gualli@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>ricardo.paredes@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>andrea.herrera@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>jose.jimenez04@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>bryan.castelo@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>juan.hernandez@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>eduardo.carrion@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>andres.salazar02@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>mishell.real@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>lenin.mino@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>brandon.toapanta@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>oscar.castillo@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>ronny.amores@epn.edu.ec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jonathan.largo@epn.edu.ec </t>
+  </si>
+  <si>
+    <t>jessica.gualpa@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>edwin.guamushig@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>andres.paredes01@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>jonathan.vilatuna@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>romina.trujillo@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>bryan.mosquera@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>leandro.ponce@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>erick.perez01@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>hugo.moncayo@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>samir.zurita@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>jonathan.zea@epn.edu.ec</t>
+  </si>
+  <si>
+    <t>Marco E. Benalcázar</t>
+  </si>
+  <si>
+    <t>Lorena Barona</t>
+  </si>
+  <si>
+    <t>Leonardo Valdivieso</t>
+  </si>
+  <si>
+    <t>Jonathan Zea</t>
+  </si>
+  <si>
+    <t>Francis Ferri</t>
+  </si>
+  <si>
+    <t>Victor Vimos</t>
+  </si>
+  <si>
+    <t>Juan Pablo Vasconez</t>
+  </si>
+  <si>
+    <t>Alex Chico</t>
+  </si>
+  <si>
+    <t>Danny Díaz</t>
+  </si>
+  <si>
+    <t>Ricardo Romero</t>
+  </si>
+  <si>
+    <t>Jeimmy eche</t>
+  </si>
+  <si>
+    <t>Sergio guaman</t>
+  </si>
+  <si>
+    <t>Verónica zúñiga</t>
+  </si>
+  <si>
+    <t>Anthony plua</t>
+  </si>
+  <si>
+    <t>Byron ortiz</t>
+  </si>
+  <si>
+    <t>Diego arias</t>
+  </si>
+  <si>
+    <t>Jorge martínez</t>
+  </si>
+  <si>
+    <t>Pablo flores</t>
+  </si>
+  <si>
+    <t>Ivanna cevallos</t>
+  </si>
+  <si>
+    <t>Kharol chicaiza</t>
+  </si>
+  <si>
+    <t>Dayana guacapiña</t>
+  </si>
+  <si>
+    <t>Jonathan gualli</t>
+  </si>
+  <si>
+    <t>Ricardo paredes</t>
+  </si>
+  <si>
+    <t>Andrea herrera</t>
+  </si>
+  <si>
+    <t>José jiménez</t>
+  </si>
+  <si>
+    <t>Bryan castelo</t>
+  </si>
+  <si>
+    <t>Juan hernández</t>
+  </si>
+  <si>
+    <t>Eduardo carrion</t>
+  </si>
+  <si>
+    <t>Andres salazar</t>
+  </si>
+  <si>
+    <t>Mishell real</t>
+  </si>
+  <si>
+    <t>Lenin miño</t>
+  </si>
+  <si>
+    <t>Brandon toapanta</t>
+  </si>
+  <si>
+    <t>Oscar castillo</t>
+  </si>
+  <si>
+    <t>Ronny amores</t>
+  </si>
+  <si>
+    <t>Jonathan largo</t>
+  </si>
+  <si>
+    <t>Jessica gualpa</t>
+  </si>
+  <si>
+    <t>Edwin guamushig</t>
+  </si>
+  <si>
+    <t>Andres paredes</t>
+  </si>
+  <si>
+    <t>Jonathan vilatuña</t>
+  </si>
+  <si>
+    <t>Romina trujillo</t>
+  </si>
+  <si>
+    <t>Bryan mosquera</t>
+  </si>
+  <si>
+    <t>Leandro ponce</t>
+  </si>
+  <si>
+    <t>Erick pérez</t>
+  </si>
+  <si>
+    <t>Hugo moncayo</t>
+  </si>
+  <si>
+    <t>Samir zurita</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -191,29 +355,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -492,198 +640,717 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="56.85546875" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>37</v>
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>5930000000</v>
+      </c>
+      <c r="D3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4">
+        <v>5930000000</v>
+      </c>
+      <c r="D4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>5930000000</v>
+      </c>
+      <c r="D5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6">
+        <v>5930000000</v>
+      </c>
+      <c r="D6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>5930000000</v>
+      </c>
+      <c r="D7" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>5930000000</v>
+      </c>
+      <c r="D8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>5930000000</v>
+      </c>
+      <c r="D9" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>5930000000</v>
+      </c>
+      <c r="D10" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>5930000000</v>
+      </c>
+      <c r="D11" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>5930000000</v>
+      </c>
+      <c r="D12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>5930000000</v>
+      </c>
+      <c r="D13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <v>5930000000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>5930000000</v>
+      </c>
+      <c r="D15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>5930000000</v>
+      </c>
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17">
+        <v>5930000000</v>
+      </c>
+      <c r="D17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18">
+        <v>5930000000</v>
+      </c>
+      <c r="D18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19">
+        <v>5930000000</v>
+      </c>
+      <c r="D19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20">
+        <v>5930000000</v>
+      </c>
+      <c r="D20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C21">
+        <v>5930000000</v>
+      </c>
+      <c r="D21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22">
+        <v>5930000000</v>
+      </c>
+      <c r="D22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C23">
+        <v>5930000000</v>
+      </c>
+      <c r="D23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24">
+        <v>5930000000</v>
+      </c>
+      <c r="D24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25">
+        <v>5930000000</v>
+      </c>
+      <c r="D25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26">
+        <v>5930000000</v>
+      </c>
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27">
+        <v>5930000000</v>
+      </c>
+      <c r="D27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28">
+        <v>5930000000</v>
+      </c>
+      <c r="D28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="C29">
+        <v>5930000000</v>
+      </c>
+      <c r="D29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30">
+        <v>5930000000</v>
+      </c>
+      <c r="D30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31">
+        <v>5930000000</v>
+      </c>
+      <c r="D31" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32">
+        <v>5930000000</v>
+      </c>
+      <c r="D32" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33">
+        <v>5930000000</v>
+      </c>
+      <c r="D33" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34">
+        <v>5930000000</v>
+      </c>
+      <c r="D34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35">
+        <v>5930000000</v>
+      </c>
+      <c r="D35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36">
+        <v>5930000000</v>
+      </c>
+      <c r="D36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37">
+        <v>5930000000</v>
+      </c>
+      <c r="D37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38">
+        <v>5930000000</v>
+      </c>
+      <c r="D38" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39">
+        <v>5930000000</v>
+      </c>
+      <c r="D39" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40">
+        <v>5930000000</v>
+      </c>
+      <c r="D40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41">
+        <v>5930000000</v>
+      </c>
+      <c r="D41" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42">
+        <v>5930000000</v>
+      </c>
+      <c r="D42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43">
+        <v>5930000000</v>
+      </c>
+      <c r="D43" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44">
+        <v>5930000000</v>
+      </c>
+      <c r="D44" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45">
+        <v>5930000000</v>
+      </c>
+      <c r="D45" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46">
+        <v>5930000000</v>
+      </c>
+      <c r="D46" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47">
+        <v>5930000000</v>
+      </c>
+      <c r="D47" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{8BD40952-1AF5-4728-A055-B23B8F6F34D3}"/>
     <hyperlink ref="B6" r:id="rId2" xr:uid="{A75EFE50-A6A3-4751-960D-30DE377C7AF2}"/>
     <hyperlink ref="B8" r:id="rId3" xr:uid="{5A6A673A-F807-4392-AB3D-53386085A02B}"/>
     <hyperlink ref="B9" r:id="rId4" xr:uid="{3F272052-19AB-4259-9A3F-9B9E950F177A}"/>
     <hyperlink ref="B11" r:id="rId5" xr:uid="{C4801EF3-5848-4AF1-95CD-892953B6FC13}"/>
+    <hyperlink ref="B13" r:id="rId6" display="mailto:jeimmy.eche@epn.edu.ec" xr:uid="{B37EDBA0-0E4E-4453-94B0-2F6B527EDB70}"/>
+    <hyperlink ref="B14" r:id="rId7" display="mailto:sergio.guaman@epn.edu.ec" xr:uid="{610D2B19-3240-4D69-B228-4331ABD495E4}"/>
+    <hyperlink ref="B15" r:id="rId8" display="mailto:veronica.zuniga@epn.edu.ec" xr:uid="{43E56B6A-D902-41D7-AFA8-02D1B9E3C654}"/>
+    <hyperlink ref="B16" r:id="rId9" display="mailto:anthony.plua@epn.edu.ec" xr:uid="{8A84C4DA-8FAE-4EAF-A65B-5DC639253431}"/>
+    <hyperlink ref="B17" r:id="rId10" display="mailto:byron.ortiz@epn.edu.ec" xr:uid="{44F8B3FB-4CDE-45CB-ABD6-9555262622C6}"/>
+    <hyperlink ref="B18" r:id="rId11" display="mailto:diego.arias@epn.edu.ec" xr:uid="{CE295EFF-56DB-409F-A181-A842A09C0865}"/>
+    <hyperlink ref="B19" r:id="rId12" display="mailto:oscar.castillo@epn.edu.ec" xr:uid="{1236F5F5-F90E-4052-82A9-4725666B1AD5}"/>
+    <hyperlink ref="B20" r:id="rId13" xr:uid="{E343EB1C-F36F-42BE-86AB-C3CA013D2685}"/>
+    <hyperlink ref="B28" r:id="rId14" xr:uid="{A2356275-4B7F-43DE-8B15-214B7E968E7F}"/>
+    <hyperlink ref="B29" r:id="rId15" xr:uid="{50C3FD4F-A26F-4E1A-B23E-08F292C48A23}"/>
+    <hyperlink ref="B21" r:id="rId16" display="mailto:ivanna.cevallos@epn.edu.ec" xr:uid="{774BC6FC-0F64-415F-A6C9-838149349965}"/>
+    <hyperlink ref="B22" r:id="rId17" display="mailto:kharol.chicaiza@epn.edu.ec" xr:uid="{ABCF326D-E044-4E4E-BEAB-52949EB742D2}"/>
+    <hyperlink ref="B23" r:id="rId18" display="mailto:dayana.guacapina@epn.edu.ec" xr:uid="{B3972476-12FF-411A-AA8E-4A312C03B54B}"/>
+    <hyperlink ref="B24" r:id="rId19" display="mailto:jonathan.gualli@epn.edu.ec" xr:uid="{FF287A7B-FE88-42CF-89A5-AABE8E8BF338}"/>
+    <hyperlink ref="B25" r:id="rId20" display="mailto:ricardo.paredes@epn.edu.ec" xr:uid="{DAAD4F94-1DB1-4297-9794-F04976CD2E2A}"/>
+    <hyperlink ref="B26" r:id="rId21" display="mailto:andrea.herrera@epn.edu.ec" xr:uid="{C2069ACE-30FB-47F5-9F44-875EA6CF753B}"/>
+    <hyperlink ref="B27" r:id="rId22" display="mailto:jose.jimenez04@epn.edu.ec" xr:uid="{541BDBFA-8B64-4108-ADB7-9A2BA94D0CDA}"/>
+    <hyperlink ref="B33" r:id="rId23" xr:uid="{7ED61069-D4F5-4A83-977B-7679D0A2F973}"/>
+    <hyperlink ref="B43" r:id="rId24" xr:uid="{73D45AE3-7AD5-490D-AB5F-BDED9E604C32}"/>
+    <hyperlink ref="B44" r:id="rId25" xr:uid="{DB7F4EDA-9B90-4A7A-A4B3-52AE95094C4C}"/>
+    <hyperlink ref="B39" r:id="rId26" xr:uid="{C9A75860-17DD-4455-9621-B38E4282EC00}"/>
+    <hyperlink ref="B41" r:id="rId27" xr:uid="{71153000-ADC0-464F-9F46-AE95A7D8061B}"/>
+    <hyperlink ref="B37" r:id="rId28" xr:uid="{707128FC-9FFB-4F0B-B0D6-CED492F86AF5}"/>
+    <hyperlink ref="B35" r:id="rId29" display="mailto:oscar.castillo@epn.edu.ec" xr:uid="{FB53734F-3FA3-45AC-8109-2B406BBF8F20}"/>
+    <hyperlink ref="B36" r:id="rId30" display="mailto:ronny.amores@epn.edu.ec" xr:uid="{BBEEC465-BBDF-4A6A-A940-6C7ED780B99C}"/>
+    <hyperlink ref="B38" r:id="rId31" display="mailto:jessica.gualpa@epn.edu.ec" xr:uid="{AB8A1F80-82AA-4EB4-91C0-96F17A1B8344}"/>
+    <hyperlink ref="B45" r:id="rId32" display="mailto:erick.perez01@epn.edu.ec" xr:uid="{4EBD337D-03EC-43EF-B25B-DF3F6E0FA111}"/>
+    <hyperlink ref="B42" r:id="rId33" display="mailto:romina.trujillo@epn.edu.ec" xr:uid="{419386B0-9C94-452B-A5D6-4EF0FC4BC014}"/>
+    <hyperlink ref="B47" r:id="rId34" display="mailto:samir.zurita@epn.edu.ec" xr:uid="{E2D29C52-E6F6-474A-AA73-203F07431B46}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId35"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Improving GUI and gifs.
</commit_message>
<xml_diff>
--- a/configs/Investigadores y Ayudantes.xlsx
+++ b/configs/Investigadores y Ayudantes.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3546FC-1524-4691-8802-ED6F73D9CF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0868F2-0AB2-449B-84F0-ED89FA80BB65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="870" yWindow="-120" windowWidth="28050" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="59">
   <si>
     <t>Nombre</t>
   </si>
@@ -185,6 +185,18 @@
   </si>
   <si>
     <t>mail</t>
+  </si>
+  <si>
+    <t>Bryan Flores</t>
+  </si>
+  <si>
+    <t>César León</t>
+  </si>
+  <si>
+    <t>Miguel Muñoz</t>
+  </si>
+  <si>
+    <t>Oscar Rivera</t>
   </si>
 </sst>
 </file>
@@ -226,8 +238,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,29 +523,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49:D52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="56.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -538,13 +555,13 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -552,13 +569,13 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3">
-        <v>5930000000</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -566,13 +583,13 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4">
-        <v>5930000000</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -580,13 +597,13 @@
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5">
-        <v>5930000000</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -594,13 +611,13 @@
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6">
-        <v>5930000000</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -608,13 +625,13 @@
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7">
-        <v>5930000000</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -622,13 +639,13 @@
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8">
-        <v>5930000000</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -636,13 +653,13 @@
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9">
-        <v>5930000000</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -650,13 +667,13 @@
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10">
-        <v>5930000000</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="B10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -664,13 +681,13 @@
       <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11">
-        <v>5930000000</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -678,13 +695,13 @@
       <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12">
-        <v>5930000000</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -692,13 +709,13 @@
       <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13">
-        <v>5930000000</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="B13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -706,13 +723,13 @@
       <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="B14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14">
-        <v>5930000000</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="B14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -720,13 +737,13 @@
       <c r="A15" t="s">
         <v>20</v>
       </c>
-      <c r="B15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15">
-        <v>5930000000</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="B15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -734,13 +751,13 @@
       <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="B16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16">
-        <v>5930000000</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="B16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -748,13 +765,13 @@
       <c r="A17" t="s">
         <v>22</v>
       </c>
-      <c r="B17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17">
-        <v>5930000000</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="B17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -762,13 +779,13 @@
       <c r="A18" t="s">
         <v>23</v>
       </c>
-      <c r="B18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18">
-        <v>5930000000</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="B18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -776,13 +793,13 @@
       <c r="A19" t="s">
         <v>24</v>
       </c>
-      <c r="B19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19">
-        <v>5930000000</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="B19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -790,13 +807,13 @@
       <c r="A20" t="s">
         <v>25</v>
       </c>
-      <c r="B20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20">
-        <v>5930000000</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="B20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -804,13 +821,13 @@
       <c r="A21" t="s">
         <v>26</v>
       </c>
-      <c r="B21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21">
-        <v>5930000000</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="B21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -818,13 +835,13 @@
       <c r="A22" t="s">
         <v>27</v>
       </c>
-      <c r="B22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22">
-        <v>5930000000</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="B22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -832,13 +849,13 @@
       <c r="A23" t="s">
         <v>28</v>
       </c>
-      <c r="B23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23">
-        <v>5930000000</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="B23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -846,13 +863,13 @@
       <c r="A24" t="s">
         <v>29</v>
       </c>
-      <c r="B24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24">
-        <v>5930000000</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="B24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -860,13 +877,13 @@
       <c r="A25" t="s">
         <v>30</v>
       </c>
-      <c r="B25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25">
-        <v>5930000000</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="B25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -874,13 +891,13 @@
       <c r="A26" t="s">
         <v>31</v>
       </c>
-      <c r="B26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26">
-        <v>5930000000</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="B26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -888,13 +905,13 @@
       <c r="A27" t="s">
         <v>32</v>
       </c>
-      <c r="B27" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27">
-        <v>5930000000</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="B27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -902,13 +919,13 @@
       <c r="A28" t="s">
         <v>33</v>
       </c>
-      <c r="B28" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28">
-        <v>5930000000</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="B28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -916,13 +933,13 @@
       <c r="A29" t="s">
         <v>34</v>
       </c>
-      <c r="B29" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29">
-        <v>5930000000</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="B29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -930,13 +947,13 @@
       <c r="A30" t="s">
         <v>35</v>
       </c>
-      <c r="B30" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30">
-        <v>5930000000</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="B30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -944,13 +961,13 @@
       <c r="A31" t="s">
         <v>36</v>
       </c>
-      <c r="B31" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31">
-        <v>5930000000</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="B31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -958,13 +975,13 @@
       <c r="A32" t="s">
         <v>37</v>
       </c>
-      <c r="B32" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32">
-        <v>5930000000</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="B32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -972,13 +989,13 @@
       <c r="A33" t="s">
         <v>38</v>
       </c>
-      <c r="B33" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33">
-        <v>5930000000</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="B33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -986,13 +1003,13 @@
       <c r="A34" t="s">
         <v>39</v>
       </c>
-      <c r="B34" t="s">
-        <v>54</v>
-      </c>
-      <c r="C34">
-        <v>5930000000</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="B34" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1000,13 +1017,13 @@
       <c r="A35" t="s">
         <v>40</v>
       </c>
-      <c r="B35" t="s">
-        <v>54</v>
-      </c>
-      <c r="C35">
-        <v>5930000000</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="B35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1014,13 +1031,13 @@
       <c r="A36" t="s">
         <v>41</v>
       </c>
-      <c r="B36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C36">
-        <v>5930000000</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="B36" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1028,13 +1045,13 @@
       <c r="A37" t="s">
         <v>42</v>
       </c>
-      <c r="B37" t="s">
-        <v>54</v>
-      </c>
-      <c r="C37">
-        <v>5930000000</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="B37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1042,13 +1059,13 @@
       <c r="A38" t="s">
         <v>43</v>
       </c>
-      <c r="B38" t="s">
-        <v>54</v>
-      </c>
-      <c r="C38">
-        <v>5930000000</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="B38" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1056,13 +1073,13 @@
       <c r="A39" t="s">
         <v>44</v>
       </c>
-      <c r="B39" t="s">
-        <v>54</v>
-      </c>
-      <c r="C39">
-        <v>5930000000</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="B39" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1070,13 +1087,13 @@
       <c r="A40" t="s">
         <v>45</v>
       </c>
-      <c r="B40" t="s">
-        <v>54</v>
-      </c>
-      <c r="C40">
-        <v>5930000000</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="B40" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1084,13 +1101,13 @@
       <c r="A41" t="s">
         <v>46</v>
       </c>
-      <c r="B41" t="s">
-        <v>54</v>
-      </c>
-      <c r="C41">
-        <v>5930000000</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="B41" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1098,13 +1115,13 @@
       <c r="A42" t="s">
         <v>47</v>
       </c>
-      <c r="B42" t="s">
-        <v>54</v>
-      </c>
-      <c r="C42">
-        <v>5930000000</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="B42" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1112,13 +1129,13 @@
       <c r="A43" t="s">
         <v>48</v>
       </c>
-      <c r="B43" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43">
-        <v>5930000000</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="B43" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1126,13 +1143,13 @@
       <c r="A44" t="s">
         <v>49</v>
       </c>
-      <c r="B44" t="s">
-        <v>54</v>
-      </c>
-      <c r="C44">
-        <v>5930000000</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="B44" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1140,13 +1157,13 @@
       <c r="A45" t="s">
         <v>50</v>
       </c>
-      <c r="B45" t="s">
-        <v>54</v>
-      </c>
-      <c r="C45">
-        <v>5930000000</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="B45" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1154,13 +1171,13 @@
       <c r="A46" t="s">
         <v>51</v>
       </c>
-      <c r="B46" t="s">
-        <v>54</v>
-      </c>
-      <c r="C46">
-        <v>5930000000</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="B46" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1168,13 +1185,13 @@
       <c r="A47" t="s">
         <v>52</v>
       </c>
-      <c r="B47" t="s">
-        <v>54</v>
-      </c>
-      <c r="C47">
-        <v>5930000000</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="B47" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1182,13 +1199,69 @@
       <c r="A48" t="s">
         <v>53</v>
       </c>
-      <c r="B48" t="s">
-        <v>54</v>
-      </c>
-      <c r="C48">
-        <v>5930000000</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="B48" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>57</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ADDED: gif & seleccionar migration 7/10/24
</commit_message>
<xml_diff>
--- a/configs/Investigadores y Ayudantes.xlsx
+++ b/configs/Investigadores y Ayudantes.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0868F2-0AB2-449B-84F0-ED89FA80BB65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76057AF-92FD-4971-846F-61E921CD4155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="-120" windowWidth="28050" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="60">
   <si>
     <t>Nombre</t>
   </si>
@@ -197,13 +197,16 @@
   </si>
   <si>
     <t>Oscar Rivera</t>
+  </si>
+  <si>
+    <t>Alexander Motoche</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +216,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -238,9 +249,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -523,21 +537,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49:D52"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -565,7 +579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -579,7 +593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -593,7 +607,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -607,7 +621,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -621,7 +635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -635,7 +649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -649,7 +663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -663,7 +677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -677,7 +691,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -691,7 +705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -705,7 +719,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -719,7 +733,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -733,7 +747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -747,7 +761,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -761,7 +775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -775,7 +789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -789,7 +803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -803,7 +817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -817,7 +831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -831,7 +845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -845,7 +859,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -859,7 +873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -873,7 +887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -887,7 +901,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -901,7 +915,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -915,7 +929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -929,7 +943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -943,7 +957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -957,7 +971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -971,7 +985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -985,7 +999,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -999,7 +1013,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -1013,7 +1027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -1027,7 +1041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -1041,7 +1055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -1055,7 +1069,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -1069,7 +1083,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -1083,7 +1097,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -1097,7 +1111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -1111,7 +1125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -1125,7 +1139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -1139,7 +1153,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -1153,7 +1167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -1167,7 +1181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -1181,7 +1195,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -1195,7 +1209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -1209,7 +1223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -1223,7 +1237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -1237,7 +1251,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -1251,7 +1265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -1264,6 +1278,23 @@
       <c r="D52" s="1" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>59</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" s="1">
+        <v>5930000000</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D57" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>